<commit_message>
v2.1 fixed a mistake in naming convention
</commit_message>
<xml_diff>
--- a/LH_TESTCASES/LH_TC_PUBLISHARTICLE.xlsx
+++ b/LH_TESTCASES/LH_TC_PUBLISHARTICLE.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="114">
   <si>
     <t>Project name</t>
   </si>
@@ -338,10 +338,10 @@
     <t>The system display a red-colored inline error message below the title field "Title is required"</t>
   </si>
   <si>
-    <t>LH-SRS-PUBART-011</t>
-  </si>
-  <si>
-    <t>Allow form submission when the article body is under 1000 words</t>
+    <t>LH-SRS-PUBART-012</t>
+  </si>
+  <si>
+    <t>Validate form submission when the article body is under 1000 words</t>
   </si>
   <si>
     <t>Here</t>
@@ -350,13 +350,13 @@
     <t>LH-TC-PUBART-015</t>
   </si>
   <si>
-    <t>Allow form submission when the article body is equal to 1000 words</t>
+    <t>Validate form submission when the article body is equal to 1000 words</t>
   </si>
   <si>
     <t>LH-TC-PUBART-016</t>
   </si>
   <si>
-    <t>Allow form submission when the article body is over 1000 words</t>
+    <t>Validate form submission when the article body is over 1000 words</t>
   </si>
   <si>
     <t>The system display an inline error message indicating the word limit has been exceeded</t>
@@ -400,6 +400,12 @@
   </si>
   <si>
     <t>Separated and modified Publish Article Test cases according to the latest updated SRS</t>
+  </si>
+  <si>
+    <t>v2.1</t>
+  </si>
+  <si>
+    <t>fixed a mistake in naming convention</t>
   </si>
 </sst>
 </file>
@@ -413,7 +419,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -518,13 +524,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -652,7 +651,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -673,12 +672,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -722,12 +715,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1109,16 +1096,16 @@
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1127,7 +1114,10 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1136,37 +1126,37 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1178,13 +1168,16 @@
     <xf numFmtId="0" fontId="30" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1193,10 +1186,10 @@
     <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1205,10 +1198,10 @@
     <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1217,10 +1210,10 @@
     <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1229,10 +1222,10 @@
     <xf numFmtId="0" fontId="31" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1241,13 +1234,7 @@
     <xf numFmtId="0" fontId="31" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1331,7 +1318,7 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1769,15 +1756,15 @@
   <sheetPr/>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25:J25"/>
+    <sheetView zoomScale="79" zoomScaleNormal="79" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21"/>
   <cols>
     <col min="1" max="1" width="31" style="16" customWidth="1"/>
     <col min="2" max="2" width="28" style="17" customWidth="1"/>
-    <col min="3" max="3" width="56.2857142857143" style="17" customWidth="1"/>
+    <col min="3" max="3" width="59.8571428571429" style="17" customWidth="1"/>
     <col min="4" max="4" width="57.7333333333333" style="18" customWidth="1"/>
     <col min="5" max="5" width="71.4285714285714" style="19" customWidth="1"/>
     <col min="6" max="6" width="37.9619047619048" style="20" customWidth="1"/>
@@ -2384,7 +2371,7 @@
       <c r="I26" s="55"/>
       <c r="J26" s="45"/>
     </row>
-    <row r="27" ht="15.75" spans="1:10">
+    <row r="27" spans="1:10">
       <c r="A27" s="39"/>
       <c r="B27" s="39"/>
       <c r="C27" s="38"/>
@@ -2526,7 +2513,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9 I10 I11 I12 I13 I20 I21 I24 I25 I14:I19 I22:I23 I26:I1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9:I1048576">
       <formula1>"Pass, Fail, Blocked, N/A"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2547,7 +2534,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="3"/>
@@ -2629,11 +2616,20 @@
         <v>45788</v>
       </c>
     </row>
-    <row r="6" s="3" customFormat="1" spans="1:4">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
+    <row r="6" s="3" customFormat="1" ht="21" spans="1:4">
+      <c r="A6" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="10">
+        <f>DATE(2025,5,11)</f>
+        <v>45788</v>
+      </c>
     </row>
     <row r="7" s="4" customFormat="1" ht="15.75" spans="1:4">
       <c r="A7" s="11"/>

</xml_diff>